<commit_message>
Re-ran NC & SC
</commit_message>
<xml_diff>
--- a/analysis/NC/NC2022-rv-points.xlsx
+++ b/analysis/NC/NC2022-rv-points.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2309E73F-42BD-D748-8757-71BA69AE1D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0FEB24E-3DDE-7243-B5BD-F9B55C583F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="500" windowWidth="27280" windowHeight="16940" xr2:uid="{C99B7473-B2A6-F045-847B-1C9C756803B7}"/>
+    <workbookView xWindow="1480" yWindow="1000" windowWidth="26940" windowHeight="16440" xr2:uid="{DF693A26-542E-2E4E-8B53-7BC12CF531B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{0A0C3A4E-CC3A-BD43-8DD7-2554E3D3BBA1}" name="NC2022-vi-points" type="6" refreshedVersion="8" background="1" saveData="1">
+  <connection id="1" xr16:uid="{C6A1434A-4A4B-A84A-AC8A-1CA3488580FE}" name="NC2022-vi-points" type="6" refreshedVersion="8" background="1" saveData="1">
     <textPr codePage="10000" sourceFile="/Users/alecramsay/dev/method_eval/data/NC/NC2022-vi-points.csv" comma="1">
       <textFields count="14">
         <textField/>
@@ -64,7 +64,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>CD</t>
+  </si>
   <si>
     <t>composite</t>
   </si>
@@ -81,6 +84,12 @@
     <t>S2016</t>
   </si>
   <si>
+    <t>G2020</t>
+  </si>
+  <si>
+    <t>AG2020</t>
+  </si>
+  <si>
     <t>MEAN</t>
   </si>
   <si>
@@ -90,15 +99,6 @@
     <t>RSE</t>
   </si>
   <si>
-    <t>Rank</t>
-  </si>
-  <si>
-    <t>G2018</t>
-  </si>
-  <si>
-    <t>AG2018</t>
-  </si>
-  <si>
     <t>Δ</t>
   </si>
   <si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Δ/SEM</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
   <si>
     <t>Average</t>
@@ -181,7 +184,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="NC2022-vi-points" connectionId="1" xr16:uid="{17A7228E-7E7F-4741-BB24-0850785186E4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="NC2022-vi-points" connectionId="1" xr16:uid="{EEBED9B2-AB32-5A4A-8124-40D9AFF2737B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -480,57 +483,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7CD971-3AE1-5D46-92D6-695D9C0B40DF}">
-  <dimension ref="A1:N20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA512FA-4585-7E48-8DC8-D1294C182B8D}">
+  <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:A15"/>
+      <selection pane="bottomRight" activeCell="I17" sqref="I17:N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="11" width="9.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="14" width="9.83203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>11</v>
@@ -541,10 +544,13 @@
       <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3">
         <v>0.30952200000000002</v>
@@ -586,9 +592,9 @@
         <v>0.166773</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3">
         <v>0.33267400000000003</v>
@@ -630,7 +636,7 @@
         <v>0.19209499999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -674,9 +680,9 @@
         <v>0.128827</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3">
         <v>0.39757700000000001</v>
@@ -718,9 +724,9 @@
         <v>0.13532</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" s="3">
         <v>0.44512000000000002</v>
@@ -729,7 +735,7 @@
         <v>0.43554100000000001</v>
       </c>
       <c r="D6" s="3">
-        <v>0.420572</v>
+        <v>0.43303999999999998</v>
       </c>
       <c r="E6" s="3">
         <v>0.43970599999999999</v>
@@ -744,27 +750,27 @@
         <v>0.45327400000000001</v>
       </c>
       <c r="I6" s="3">
-        <v>0.44214900000000001</v>
+        <v>0.44422699999999998</v>
       </c>
       <c r="J6" s="3">
-        <v>7.8189999999999996E-3</v>
+        <v>6.8929999999999998E-3</v>
       </c>
       <c r="K6" s="3">
-        <v>1.7683999999999998E-2</v>
+        <v>1.5517E-2</v>
       </c>
       <c r="L6" s="3">
-        <v>2.9710000000000001E-3</v>
+        <v>8.9300000000000002E-4</v>
       </c>
       <c r="M6" s="3">
-        <v>6.7190000000000001E-3</v>
+        <v>2.0100000000000001E-3</v>
       </c>
       <c r="N6" s="3">
-        <v>0.37997199999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.129552</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B7" s="3">
         <v>0.450158</v>
@@ -773,7 +779,7 @@
         <v>0.44851600000000003</v>
       </c>
       <c r="D7" s="3">
-        <v>0.43303999999999998</v>
+        <v>0.420572</v>
       </c>
       <c r="E7" s="3">
         <v>0.45153599999999999</v>
@@ -788,27 +794,27 @@
         <v>0.456403</v>
       </c>
       <c r="I7" s="3">
-        <v>0.45066800000000001</v>
+        <v>0.44858999999999999</v>
       </c>
       <c r="J7" s="3">
-        <v>6.9329999999999999E-3</v>
+        <v>8.1880000000000008E-3</v>
       </c>
       <c r="K7" s="3">
-        <v>1.5384E-2</v>
+        <v>1.8252999999999998E-2</v>
       </c>
       <c r="L7" s="3">
-        <v>-5.1000000000000004E-4</v>
+        <v>1.5679999999999999E-3</v>
       </c>
       <c r="M7" s="3">
-        <v>-1.132E-3</v>
+        <v>3.4949999999999998E-3</v>
       </c>
       <c r="N7" s="3">
-        <v>-7.3561000000000001E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.1915</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3">
         <v>0.46771200000000002</v>
@@ -850,9 +856,9 @@
         <v>0.12285799999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3">
         <v>0.50668400000000002</v>
@@ -894,9 +900,9 @@
         <v>0.18251200000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B10" s="3">
         <v>0.54930699999999999</v>
@@ -911,7 +917,7 @@
         <v>0.54400000000000004</v>
       </c>
       <c r="F10" s="3">
-        <v>0.51078400000000002</v>
+        <v>0.54363499999999998</v>
       </c>
       <c r="G10" s="3">
         <v>0.56405000000000005</v>
@@ -920,33 +926,33 @@
         <v>0.55621100000000001</v>
       </c>
       <c r="I10" s="3">
-        <v>0.54374</v>
+        <v>0.54921500000000001</v>
       </c>
       <c r="J10" s="3">
-        <v>7.6340000000000002E-3</v>
+        <v>4.0090000000000004E-3</v>
       </c>
       <c r="K10" s="3">
-        <v>1.404E-2</v>
+        <v>7.3000000000000001E-3</v>
       </c>
       <c r="L10" s="3">
-        <v>5.5669999999999999E-3</v>
+        <v>9.2E-5</v>
       </c>
       <c r="M10" s="3">
-        <v>1.0238000000000001E-2</v>
+        <v>1.6799999999999999E-4</v>
       </c>
       <c r="N10" s="3">
-        <v>0.72923800000000005</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+        <v>2.2948E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B11" s="3">
         <v>0.56353900000000001</v>
       </c>
       <c r="C11" s="3">
-        <v>0.56276099999999996</v>
+        <v>0.583229</v>
       </c>
       <c r="D11" s="3">
         <v>0.55118699999999998</v>
@@ -955,42 +961,42 @@
         <v>0.55614699999999995</v>
       </c>
       <c r="F11" s="3">
-        <v>0.53812000000000004</v>
+        <v>0.51078400000000002</v>
       </c>
       <c r="G11" s="3">
-        <v>0.59578799999999998</v>
+        <v>0.59753900000000004</v>
       </c>
       <c r="H11" s="3">
-        <v>0.56822300000000003</v>
+        <v>0.56935800000000003</v>
       </c>
       <c r="I11" s="3">
-        <v>0.56203800000000004</v>
+        <v>0.56137400000000004</v>
       </c>
       <c r="J11" s="3">
-        <v>7.9629999999999996E-3</v>
+        <v>1.2300999999999999E-2</v>
       </c>
       <c r="K11" s="3">
-        <v>1.4168E-2</v>
+        <v>2.1912000000000001E-2</v>
       </c>
       <c r="L11" s="3">
-        <v>1.5009999999999999E-3</v>
+        <v>2.1649999999999998E-3</v>
       </c>
       <c r="M11" s="3">
-        <v>2.6710000000000002E-3</v>
+        <v>3.8570000000000002E-3</v>
       </c>
       <c r="N11" s="3">
-        <v>0.188497</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.17600199999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B12" s="3">
         <v>0.56432300000000002</v>
       </c>
       <c r="C12" s="3">
-        <v>0.583229</v>
+        <v>0.56276099999999996</v>
       </c>
       <c r="D12" s="3">
         <v>0.55420100000000005</v>
@@ -999,36 +1005,36 @@
         <v>0.56275600000000003</v>
       </c>
       <c r="F12" s="3">
-        <v>0.54363499999999998</v>
+        <v>0.53812000000000004</v>
       </c>
       <c r="G12" s="3">
-        <v>0.59753900000000004</v>
+        <v>0.59578799999999998</v>
       </c>
       <c r="H12" s="3">
-        <v>0.56935800000000003</v>
+        <v>0.56822300000000003</v>
       </c>
       <c r="I12" s="3">
-        <v>0.56845299999999999</v>
+        <v>0.56364199999999998</v>
       </c>
       <c r="J12" s="3">
-        <v>7.9930000000000001E-3</v>
+        <v>7.7380000000000001E-3</v>
       </c>
       <c r="K12" s="3">
-        <v>1.4061000000000001E-2</v>
+        <v>1.3729E-2</v>
       </c>
       <c r="L12" s="3">
-        <v>-4.13E-3</v>
+        <v>6.8099999999999996E-4</v>
       </c>
       <c r="M12" s="3">
-        <v>-7.2649999999999998E-3</v>
+        <v>1.2080000000000001E-3</v>
       </c>
       <c r="N12" s="3">
-        <v>-0.51670199999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+        <v>8.8007000000000002E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B13" s="3">
         <v>0.63153899999999996</v>
@@ -1046,33 +1052,33 @@
         <v>0.57678600000000002</v>
       </c>
       <c r="G13" s="3">
-        <v>0.67162900000000003</v>
+        <v>0.67297099999999999</v>
       </c>
       <c r="H13" s="3">
         <v>0.64183100000000004</v>
       </c>
       <c r="I13" s="3">
-        <v>0.62910900000000003</v>
+        <v>0.629332</v>
       </c>
       <c r="J13" s="3">
-        <v>1.3174999999999999E-2</v>
+        <v>1.332E-2</v>
       </c>
       <c r="K13" s="3">
-        <v>2.0941999999999999E-2</v>
+        <v>2.1165E-2</v>
       </c>
       <c r="L13" s="3">
-        <v>2.4299999999999999E-3</v>
+        <v>2.2070000000000002E-3</v>
       </c>
       <c r="M13" s="3">
-        <v>3.8630000000000001E-3</v>
+        <v>3.5070000000000001E-3</v>
       </c>
       <c r="N13" s="3">
-        <v>0.18443999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.165691</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="3">
         <v>0.64398100000000003</v>
@@ -1090,33 +1096,33 @@
         <v>0.61014999999999997</v>
       </c>
       <c r="G14" s="3">
-        <v>0.67297099999999999</v>
+        <v>0.67162900000000003</v>
       </c>
       <c r="H14" s="3">
         <v>0.650926</v>
       </c>
       <c r="I14" s="3">
-        <v>0.64283699999999999</v>
+        <v>0.64261400000000002</v>
       </c>
       <c r="J14" s="3">
-        <v>8.8389999999999996E-3</v>
+        <v>8.6879999999999995E-3</v>
       </c>
       <c r="K14" s="3">
-        <v>1.375E-2</v>
+        <v>1.3520000000000001E-2</v>
       </c>
       <c r="L14" s="3">
-        <v>1.1440000000000001E-3</v>
+        <v>1.3669999999999999E-3</v>
       </c>
       <c r="M14" s="3">
-        <v>1.7799999999999999E-3</v>
+        <v>2.127E-3</v>
       </c>
       <c r="N14" s="3">
-        <v>0.12942600000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.15734300000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B15" s="3">
         <v>0.677149</v>
@@ -1160,27 +1166,27 @@
     </row>
     <row r="17" spans="9:14" x14ac:dyDescent="0.2">
       <c r="I17" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J17" s="3">
         <f>AVERAGE(J2:J15)</f>
-        <v>7.8792857142857137E-3</v>
+        <v>7.9350714285714267E-3</v>
       </c>
       <c r="K17" s="3">
         <f t="shared" ref="K17:N17" si="0">AVERAGE(K2:K15)</f>
-        <v>1.6508000000000002E-2</v>
+        <v>1.6605642857142857E-2</v>
       </c>
       <c r="L17" s="3">
         <f t="shared" si="0"/>
-        <v>1.1647857142857139E-3</v>
+        <v>1.1647857142857141E-3</v>
       </c>
       <c r="M17" s="3">
         <f t="shared" si="0"/>
-        <v>2.5199999999999992E-3</v>
+        <v>2.4841428571428571E-3</v>
       </c>
       <c r="N17" s="3">
         <f t="shared" si="0"/>
-        <v>0.14428535714285715</v>
+        <v>0.13783771428571429</v>
       </c>
     </row>
     <row r="20" spans="9:14" x14ac:dyDescent="0.2">

</xml_diff>